<commit_message>
test jwt, change led test for tests
</commit_message>
<xml_diff>
--- a/documentation/test_reseau.xlsx
+++ b/documentation/test_reseau.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF0343-1BE6-44A6-96DD-172CD5454E08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,70 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>allumer l'univers 2 mais reste allumer</t>
+  </si>
+  <si>
+    <t>allumer l'universa 2 et 4 reste allumer</t>
+  </si>
+  <si>
+    <t>allumer unvivers 2 et 4 reste allumer</t>
+  </si>
+  <si>
+    <t>allumer unvers 2 reste allumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1 </t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test1 sync</t>
+  </si>
+  <si>
+    <t>test 2 sync</t>
+  </si>
+  <si>
+    <t>test1 continu</t>
+  </si>
+  <si>
+    <t>test1 continu sync</t>
+  </si>
+  <si>
+    <t>allumer univers 2 reste allumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 2 continue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>test 2 continue  sync</t>
+  </si>
+  <si>
+    <t>meme</t>
+  </si>
+  <si>
+    <t>Tout les tests marchent sauf que sur case chemine les leds reste allumer mais pas sur toit-vitre</t>
+  </si>
+  <si>
+    <t>pour les fad in fad out et parabole. l'animation est bizard elle reste beaucoup de temps allumer(pas sur de pouvoir employer tout les valeurs de 0 à 255)</t>
+  </si>
+  <si>
+    <t>pour la luminosité à partir de 15 16 on ne voit plus d'augmentation de la luminosité ou tres tres legerement je n'arrive pas à le voir à l'œil nu</t>
+  </si>
+  <si>
+    <t>pas de différence entre le art sync et le non artsync</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +393,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>